<commit_message>
fixes and new DB
</commit_message>
<xml_diff>
--- a/GraphDB/Results.xlsx
+++ b/GraphDB/Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Размер графа</t>
   </si>
@@ -35,37 +35,28 @@
     <t>Найденный критерий</t>
   </si>
   <si>
-    <t>114ms</t>
-  </si>
-  <si>
-    <t>74ms</t>
-  </si>
-  <si>
-    <t>1ms</t>
-  </si>
-  <si>
-    <t>2ms</t>
-  </si>
-  <si>
-    <t>3ms</t>
-  </si>
-  <si>
-    <t>238ms</t>
-  </si>
-  <si>
-    <t>201ms</t>
-  </si>
-  <si>
-    <t>29012ms</t>
-  </si>
-  <si>
-    <t>29288ms</t>
-  </si>
-  <si>
-    <t>281262ms</t>
-  </si>
-  <si>
-    <t>303738ms</t>
+    <t>0s</t>
+  </si>
+  <si>
+    <t>0,01s</t>
+  </si>
+  <si>
+    <t>0,26s</t>
+  </si>
+  <si>
+    <t>0,2s</t>
+  </si>
+  <si>
+    <t>30,43s</t>
+  </si>
+  <si>
+    <t>31,2s</t>
+  </si>
+  <si>
+    <t>291,87s</t>
+  </si>
+  <si>
+    <t>286,46s</t>
   </si>
   <si>
     <t>Spire.XLS for .NET</t>
@@ -584,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -616,7 +607,7 @@
     </row>
     <row r="2" spans="1:5" ht="12.75">
       <c r="A2">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -633,13 +624,13 @@
     </row>
     <row r="3" spans="1:5" ht="12.75">
       <c r="A3">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -650,13 +641,13 @@
     </row>
     <row r="4" spans="1:5" ht="12.75">
       <c r="A4">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0.5</v>
@@ -667,13 +658,13 @@
     </row>
     <row r="5" spans="1:5" ht="12.75">
       <c r="A5">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -684,13 +675,13 @@
     </row>
     <row r="6" spans="1:5" ht="12.75">
       <c r="A6">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>0.5</v>
@@ -701,13 +692,13 @@
     </row>
     <row r="7" spans="1:5" ht="12.75">
       <c r="A7">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0.5</v>
@@ -718,13 +709,13 @@
     </row>
     <row r="8" spans="1:5" ht="12.75">
       <c r="A8">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -735,13 +726,13 @@
     </row>
     <row r="9" spans="1:5" ht="12.75">
       <c r="A9">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>0.5</v>
@@ -752,13 +743,13 @@
     </row>
     <row r="10" spans="1:5" ht="12.75">
       <c r="A10">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>0.5</v>
@@ -769,52 +760,18 @@
     </row>
     <row r="11" spans="1:5" ht="12.75">
       <c r="A11">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>0.5</v>
       </c>
       <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75">
-      <c r="A12">
-        <v>50001</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12">
-        <v>0.5</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75">
-      <c r="A13">
-        <v>50001</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>0.5</v>
-      </c>
-      <c r="E13">
         <v>3</v>
       </c>
     </row>
@@ -863,42 +820,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>